<commit_message>
qualitative revisions before sending to alex
</commit_message>
<xml_diff>
--- a/data analysis/analysis after annotation/Phase C child reaction analysis.xlsx
+++ b/data analysis/analysis after annotation/Phase C child reaction analysis.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10538" windowHeight="4710"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6735" windowHeight="4710"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="48">
   <si>
     <t>wait for first prompt</t>
   </si>
@@ -117,6 +118,57 @@
   </si>
   <si>
     <t>CIMG1208</t>
+  </si>
+  <si>
+    <t>CIMG1214</t>
+  </si>
+  <si>
+    <t>CIMG1216</t>
+  </si>
+  <si>
+    <t>CIMG1218</t>
+  </si>
+  <si>
+    <t>CIMG1220</t>
+  </si>
+  <si>
+    <t>CIMG1223</t>
+  </si>
+  <si>
+    <t>CIMG1225</t>
+  </si>
+  <si>
+    <t>CIMG1230</t>
+  </si>
+  <si>
+    <t>2 of 3</t>
+  </si>
+  <si>
+    <t>CIMG1232</t>
+  </si>
+  <si>
+    <t>CIMG1234</t>
+  </si>
+  <si>
+    <t>CIMG1236</t>
+  </si>
+  <si>
+    <t>CIMG1238</t>
+  </si>
+  <si>
+    <t>CIMG1240</t>
+  </si>
+  <si>
+    <t>CIMG1242</t>
+  </si>
+  <si>
+    <t>3 of 4</t>
+  </si>
+  <si>
+    <t>CIMG1244</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 of 3 </t>
   </si>
 </sst>
 </file>
@@ -435,13 +487,1215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB13"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="W4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AA11" sqref="AA11"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="5" max="5" width="9.9296875" customWidth="1"/>
+    <col min="6" max="6" width="10.06640625" customWidth="1"/>
+    <col min="7" max="7" width="10.9296875" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="12.53125" customWidth="1"/>
+    <col min="10" max="10" width="10.46484375" customWidth="1"/>
+    <col min="11" max="11" width="22.19921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="37.86328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" t="s">
+        <v>5</v>
+      </c>
+      <c r="J19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" t="s">
+        <v>5</v>
+      </c>
+      <c r="J22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I26" t="s">
+        <v>5</v>
+      </c>
+      <c r="J26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" t="s">
+        <v>5</v>
+      </c>
+      <c r="I28" t="s">
+        <v>5</v>
+      </c>
+      <c r="J28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" t="s">
+        <v>8</v>
+      </c>
+      <c r="I29" t="s">
+        <v>5</v>
+      </c>
+      <c r="J29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" t="s">
+        <v>6</v>
+      </c>
+      <c r="H30" t="s">
+        <v>5</v>
+      </c>
+      <c r="I30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" t="s">
+        <v>8</v>
+      </c>
+      <c r="I31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" t="s">
+        <v>8</v>
+      </c>
+      <c r="I33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" t="s">
+        <v>6</v>
+      </c>
+      <c r="I34" t="s">
+        <v>5</v>
+      </c>
+      <c r="J34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" t="s">
+        <v>8</v>
+      </c>
+      <c r="I37" t="s">
+        <v>5</v>
+      </c>
+      <c r="J37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" t="s">
+        <v>8</v>
+      </c>
+      <c r="I38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" t="s">
+        <v>8</v>
+      </c>
+      <c r="I40" t="s">
+        <v>5</v>
+      </c>
+      <c r="J40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" t="s">
+        <v>8</v>
+      </c>
+      <c r="I42" t="s">
+        <v>5</v>
+      </c>
+      <c r="J42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" t="s">
+        <v>5</v>
+      </c>
+      <c r="F43" t="s">
+        <v>5</v>
+      </c>
+      <c r="G43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44" t="s">
+        <v>38</v>
+      </c>
+      <c r="G44" t="s">
+        <v>5</v>
+      </c>
+      <c r="I44" t="s">
+        <v>5</v>
+      </c>
+      <c r="J44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" t="s">
+        <v>5</v>
+      </c>
+      <c r="H47" t="s">
+        <v>8</v>
+      </c>
+      <c r="I47" t="s">
+        <v>8</v>
+      </c>
+      <c r="J47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" t="s">
+        <v>8</v>
+      </c>
+      <c r="G49" t="s">
+        <v>8</v>
+      </c>
+      <c r="H49" t="s">
+        <v>8</v>
+      </c>
+      <c r="I49" t="s">
+        <v>5</v>
+      </c>
+      <c r="J49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" t="s">
+        <v>5</v>
+      </c>
+      <c r="I51" t="s">
+        <v>5</v>
+      </c>
+      <c r="J51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" t="s">
+        <v>5</v>
+      </c>
+      <c r="G52" t="s">
+        <v>5</v>
+      </c>
+      <c r="H52" t="s">
+        <v>8</v>
+      </c>
+      <c r="I52" t="s">
+        <v>5</v>
+      </c>
+      <c r="J52" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53" t="s">
+        <v>5</v>
+      </c>
+      <c r="I53" t="s">
+        <v>5</v>
+      </c>
+      <c r="J53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" t="s">
+        <v>8</v>
+      </c>
+      <c r="G54" t="s">
+        <v>6</v>
+      </c>
+      <c r="H54" t="s">
+        <v>8</v>
+      </c>
+      <c r="I54" t="s">
+        <v>5</v>
+      </c>
+      <c r="J54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F55" t="s">
+        <v>45</v>
+      </c>
+      <c r="G55" t="s">
+        <v>45</v>
+      </c>
+      <c r="H55" t="s">
+        <v>5</v>
+      </c>
+      <c r="I55" t="s">
+        <v>5</v>
+      </c>
+      <c r="J55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" t="s">
+        <v>5</v>
+      </c>
+      <c r="E56" t="s">
+        <v>47</v>
+      </c>
+      <c r="F56" t="s">
+        <v>5</v>
+      </c>
+      <c r="G56" t="s">
+        <v>5</v>
+      </c>
+      <c r="H56" t="s">
+        <v>5</v>
+      </c>
+      <c r="I56" t="s">
+        <v>5</v>
+      </c>
+      <c r="J56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AJ13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="AI13" sqref="A1:AI13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -449,22 +1703,22 @@
     <col min="1" max="1" width="39.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -543,8 +1797,35 @@
       <c r="AA4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AB4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -561,13 +1842,13 @@
         <v>8</v>
       </c>
       <c r="I5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K5" t="s">
         <v>8</v>
       </c>
       <c r="M5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O5" t="s">
         <v>8</v>
@@ -587,8 +1868,23 @@
       <c r="AA5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AC5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -622,8 +1918,20 @@
       <c r="AA6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AC6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -663,8 +1971,20 @@
       <c r="AB7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AD7" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -740,8 +2060,20 @@
       <c r="AB8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AC8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -811,8 +2143,20 @@
       <c r="AB9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AC9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -874,10 +2218,22 @@
         <v>5</v>
       </c>
       <c r="AA10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -932,8 +2288,29 @@
       <c r="Z11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AA11" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -997,8 +2374,29 @@
       <c r="Z12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AA12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1061,6 +2459,12 @@
       </c>
       <c r="Z13" t="s">
         <v>8</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>